<commit_message>
update intrusion/recall scripts to include all sites
</commit_message>
<xml_diff>
--- a/Jefferson_neuropsych.xlsx
+++ b/Jefferson_neuropsych.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evsnyder/rhino_mount/home1/evsnyder/analysis/mental_health/Mental_health/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242C32CD-4692-0941-A9B8-59CA02604A3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC390EA0-6B2E-3B44-809A-A2CEFB7C1EA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25040" windowHeight="14140" xr2:uid="{84FF3F45-53C2-4048-A8C5-64ACCA6BD0B4}"/>
   </bookViews>
@@ -978,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0C5771-20FA-5145-9846-CDEA26324E94}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3618,12 +3618,8 @@
         <v>32.436098389999998</v>
       </c>
       <c r="E78" s="3"/>
-      <c r="F78" s="9">
-        <v>5</v>
-      </c>
-      <c r="G78" s="9">
-        <v>6</v>
-      </c>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
       <c r="I78" s="3" t="s">
         <v>163</v>
       </c>

</xml_diff>